<commit_message>
3 updated README.md with new content
</commit_message>
<xml_diff>
--- a/exl2json/Details.xlsx
+++ b/exl2json/Details.xlsx
@@ -11,12 +11,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Arindita Saha</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>Angula2</t>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Technology</t>
   </si>
   <si>
     <t>Kislaya Pant</t>
@@ -35,6 +38,12 @@
   </si>
   <si>
     <t>CBZ</t>
+  </si>
+  <si>
+    <t>Arindita Saha</t>
+  </si>
+  <si>
+    <t>Angular 2</t>
   </si>
   <si>
     <t>Malinikesh Agrawani</t>
@@ -106,55 +115,66 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>21.0</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>21.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>25.0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>23.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>21.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>